<commit_message>
make version info sheet empty as test sim has no version_info
</commit_message>
<xml_diff>
--- a/client/simulations/tests/points_no_data.xlsx
+++ b/client/simulations/tests/points_no_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uczmh2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uczmh2\Desktop\ap-nimbus-client\client\simulations\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="11700" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="11700" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Input Values" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Title</t>
   </si>
@@ -123,99 +123,6 @@
   </si>
   <si>
     <t>Time (ms)</t>
-  </si>
-  <si>
-    <t>ApPredict Version</t>
-  </si>
-  <si>
-    <t>37cc5a6</t>
-  </si>
-  <si>
-    <t>Chaste Version</t>
-  </si>
-  <si>
-    <t>2019.1.682dce0</t>
-  </si>
-  <si>
-    <t>Modified</t>
-  </si>
-  <si>
-    <t>Build options</t>
-  </si>
-  <si>
-    <t>GccOpt, shared libraries</t>
-  </si>
-  <si>
-    <t>OS info</t>
-  </si>
-  <si>
-    <t>Linux d09b088bdc9f 4.15.0-161-generic #169-Ubuntu SMP Fri Oct 15 13:41:54 UTC 2021 x86_64</t>
-  </si>
-  <si>
-    <t>Compiler</t>
-  </si>
-  <si>
-    <t>gcc, version b'9.3.0'</t>
-  </si>
-  <si>
-    <t>Compiler flags</t>
-  </si>
-  <si>
-    <t>-O3 -std=c++14</t>
-  </si>
-  <si>
-    <t>XSD</t>
-  </si>
-  <si>
-    <t>4.0.0</t>
-  </si>
-  <si>
-    <t>VTK</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Xerces</t>
-  </si>
-  <si>
-    <t>3.2.0</t>
-  </si>
-  <si>
-    <t>SUNDIALS</t>
-  </si>
-  <si>
-    <t>2.5.0</t>
-  </si>
-  <si>
-    <t>HDF5</t>
-  </si>
-  <si>
-    <t>1.8.16</t>
-  </si>
-  <si>
-    <t>Boost</t>
-  </si>
-  <si>
-    <t>1.65.1</t>
-  </si>
-  <si>
-    <t>PETSc</t>
-  </si>
-  <si>
-    <t>3.12.4</t>
-  </si>
-  <si>
-    <t>Parmetis</t>
-  </si>
-  <si>
-    <t>4.0.3</t>
-  </si>
-  <si>
-    <t>Ap Predict arguments</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> --pacing-freq 1 --pacing-max-time 5 --plasma-conc-high 100 --plasma-conc-low 0 --plasma-conc-count 4 --plasma-conc-logscale true --model 1</t>
   </si>
 </sst>
 </file>
@@ -807,143 +714,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B16"/>
+      <selection activeCell="A18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>